<commit_message>
Paw Care Final v1.1
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/MEDICAMENTOS_VETERINARIA.xlsx
+++ b/src/main/resources/excel/MEDICAMENTOS_VETERINARIA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quiro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Escritorio\Uni\Semestres\Semestre VI\Desarrollo Web\CODIGO\PAW-CARE-BACK\PAW-CARE-SPRINGBOOT\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAE2D95-9A4B-42F2-96C8-3811195C2331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB9BA15-DFA4-4497-9B13-6A9AEC79808F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7356" yWindow="3396" windowWidth="15684" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICAMENTOS BD FINAL" sheetId="10" r:id="rId1"/>
@@ -1990,18 +1990,18 @@
   <dimension ref="A1:E524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2083,10 +2083,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2100,10 +2100,10 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>84</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>104</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>109</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>112</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>113</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>114</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>116</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>117</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>118</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>121</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>122</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>123</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>125</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>126</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>127</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>128</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>129</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>130</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>131</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>132</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>133</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>134</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>135</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>136</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>137</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>138</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>139</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>140</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>141</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>142</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>143</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>144</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>145</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>146</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>147</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>148</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>149</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>150</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>151</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>152</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>154</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>155</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>156</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>157</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>158</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>159</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>160</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>161</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>162</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>163</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>164</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>165</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>166</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>167</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>168</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>169</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>170</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>171</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>172</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>173</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>174</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>175</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>176</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>177</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>178</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>179</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>180</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>181</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>182</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>183</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>184</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>185</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>186</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>187</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>188</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>189</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>190</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>191</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>192</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>193</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>194</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>195</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>196</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>197</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>198</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>199</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>200</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>201</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>202</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>203</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>204</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>205</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>206</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>208</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>209</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>210</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>211</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>212</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>213</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>214</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>215</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>216</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>217</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>218</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>219</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>220</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>221</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>222</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>223</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>224</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>225</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>226</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>227</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>228</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>229</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>230</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>231</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>232</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>233</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>234</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>235</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>236</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>237</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>238</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>239</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>240</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>241</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>242</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>243</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>244</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>245</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>246</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>247</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>248</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>249</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>250</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>251</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>252</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>253</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>254</v>
       </c>
@@ -6268,7 +6268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>255</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>256</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>257</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>258</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>259</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>260</v>
       </c>
@@ -6370,7 +6370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>261</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>262</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>263</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>264</v>
       </c>
@@ -6438,7 +6438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>265</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>266</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>267</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>268</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>269</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>270</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>271</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>272</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>273</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>274</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>275</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>276</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>277</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>278</v>
       </c>
@@ -6676,7 +6676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>279</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>280</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>281</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>282</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>283</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>284</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>285</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>286</v>
       </c>
@@ -6812,7 +6812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>287</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>288</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>289</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>290</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>291</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>292</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>293</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>294</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>295</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>296</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>298</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>299</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>300</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>301</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>302</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>303</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>304</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>305</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>306</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>307</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>308</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>309</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>310</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>311</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>312</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>313</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>314</v>
       </c>
@@ -7288,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>315</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>316</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>317</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>318</v>
       </c>
@@ -7356,7 +7356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>319</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>320</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>321</v>
       </c>
@@ -7407,7 +7407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>322</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>323</v>
       </c>
@@ -7441,7 +7441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>324</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>325</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>326</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>327</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>328</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>329</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>330</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>331</v>
       </c>
@@ -7577,7 +7577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>332</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>333</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>334</v>
       </c>
@@ -7628,7 +7628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>335</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>336</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>337</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>338</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>339</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>340</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>341</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>342</v>
       </c>
@@ -7764,7 +7764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>343</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>344</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>345</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>346</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>347</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>348</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>349</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>350</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>351</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>352</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>353</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>354</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>355</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>356</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>357</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>358</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>359</v>
       </c>
@@ -8053,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>360</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>361</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>362</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>363</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>364</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>365</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>366</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>367</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>368</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>369</v>
       </c>
@@ -8223,7 +8223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>370</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>371</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>372</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>373</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>374</v>
       </c>
@@ -8308,7 +8308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>375</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>376</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>377</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>378</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>379</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>380</v>
       </c>
@@ -8410,7 +8410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>381</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>382</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>383</v>
       </c>
@@ -8461,7 +8461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>384</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>385</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>386</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>387</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>388</v>
       </c>
@@ -8546,7 +8546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>389</v>
       </c>
@@ -8563,7 +8563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>390</v>
       </c>
@@ -8580,7 +8580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>391</v>
       </c>
@@ -8597,7 +8597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>392</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>393</v>
       </c>
@@ -8631,7 +8631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>394</v>
       </c>
@@ -8648,7 +8648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>395</v>
       </c>
@@ -8665,7 +8665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>396</v>
       </c>
@@ -8682,7 +8682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>397</v>
       </c>
@@ -8699,7 +8699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>398</v>
       </c>
@@ -8716,7 +8716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>399</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>400</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>401</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>402</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>403</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>404</v>
       </c>
@@ -8818,7 +8818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>405</v>
       </c>
@@ -8835,7 +8835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>406</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>407</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>408</v>
       </c>
@@ -8886,7 +8886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>409</v>
       </c>
@@ -8903,7 +8903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>410</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>411</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>412</v>
       </c>
@@ -8954,7 +8954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>413</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>414</v>
       </c>
@@ -8988,7 +8988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>415</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>416</v>
       </c>
@@ -9022,7 +9022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>417</v>
       </c>
@@ -9039,7 +9039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>418</v>
       </c>
@@ -9056,7 +9056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>419</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>420</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>421</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>422</v>
       </c>
@@ -9124,7 +9124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>423</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>424</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>425</v>
       </c>
@@ -9175,7 +9175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>426</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>427</v>
       </c>
@@ -9209,7 +9209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>428</v>
       </c>
@@ -9226,7 +9226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>429</v>
       </c>
@@ -9243,7 +9243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>430</v>
       </c>
@@ -9260,7 +9260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>431</v>
       </c>
@@ -9277,7 +9277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>432</v>
       </c>
@@ -9294,7 +9294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>433</v>
       </c>
@@ -9311,7 +9311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>434</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>435</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>436</v>
       </c>
@@ -9362,7 +9362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>437</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>438</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>439</v>
       </c>
@@ -9413,7 +9413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>440</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>441</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>442</v>
       </c>
@@ -9464,7 +9464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>443</v>
       </c>
@@ -9481,7 +9481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>444</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>445</v>
       </c>
@@ -9515,7 +9515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>446</v>
       </c>
@@ -9532,7 +9532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>447</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>448</v>
       </c>
@@ -9566,7 +9566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>449</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>450</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>451</v>
       </c>
@@ -9617,7 +9617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>452</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>453</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>454</v>
       </c>
@@ -9668,7 +9668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
         <v>455</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>456</v>
       </c>
@@ -9702,7 +9702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>457</v>
       </c>
@@ -9719,7 +9719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>458</v>
       </c>
@@ -9736,7 +9736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>459</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>460</v>
       </c>
@@ -9770,7 +9770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>461</v>
       </c>
@@ -9787,7 +9787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>462</v>
       </c>
@@ -9804,7 +9804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>463</v>
       </c>
@@ -9821,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>464</v>
       </c>
@@ -9838,7 +9838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>465</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>466</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>467</v>
       </c>
@@ -9889,7 +9889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>468</v>
       </c>
@@ -9906,7 +9906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>469</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>470</v>
       </c>
@@ -9940,7 +9940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>471</v>
       </c>
@@ -9957,7 +9957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>472</v>
       </c>
@@ -9974,7 +9974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>473</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>474</v>
       </c>
@@ -10008,7 +10008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>475</v>
       </c>
@@ -10025,7 +10025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>476</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>477</v>
       </c>
@@ -10059,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>478</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>479</v>
       </c>
@@ -10093,7 +10093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>480</v>
       </c>
@@ -10110,7 +10110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>481</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>482</v>
       </c>
@@ -10144,7 +10144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>483</v>
       </c>
@@ -10161,7 +10161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>484</v>
       </c>
@@ -10178,7 +10178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>485</v>
       </c>
@@ -10195,7 +10195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>486</v>
       </c>
@@ -10212,7 +10212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>487</v>
       </c>
@@ -10229,7 +10229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>488</v>
       </c>
@@ -10246,7 +10246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>489</v>
       </c>
@@ -10263,7 +10263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>490</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>491</v>
       </c>
@@ -10297,7 +10297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>492</v>
       </c>
@@ -10314,7 +10314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>493</v>
       </c>
@@ -10331,7 +10331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>494</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>495</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>496</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="494" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>497</v>
       </c>
@@ -10399,7 +10399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>498</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="496" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>499</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>500</v>
       </c>
@@ -10450,7 +10450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>501</v>
       </c>
@@ -10467,7 +10467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>502</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>503</v>
       </c>
@@ -10501,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>504</v>
       </c>
@@ -10518,7 +10518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>505</v>
       </c>
@@ -10535,7 +10535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>506</v>
       </c>
@@ -10552,7 +10552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>507</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="505" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>508</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>509</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>510</v>
       </c>
@@ -10620,7 +10620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="508" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>511</v>
       </c>
@@ -10637,7 +10637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="509" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>512</v>
       </c>
@@ -10654,7 +10654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="510" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>513</v>
       </c>
@@ -10671,7 +10671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>514</v>
       </c>
@@ -10688,7 +10688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="512" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>515</v>
       </c>
@@ -10705,7 +10705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>516</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>517</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>518</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>519</v>
       </c>
@@ -10773,7 +10773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>520</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A518" t="s">
         <v>521</v>
       </c>
@@ -10807,7 +10807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>522</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A520" t="s">
         <v>523</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>524</v>
       </c>
@@ -10858,7 +10858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A522" t="s">
         <v>525</v>
       </c>
@@ -10875,7 +10875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
         <v>526</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A524" t="s">
         <v>527</v>
       </c>

</xml_diff>

<commit_message>
Paw Care Final v1.2
Mejoras dashboard
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/MEDICAMENTOS_VETERINARIA.xlsx
+++ b/src/main/resources/excel/MEDICAMENTOS_VETERINARIA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Escritorio\Uni\Semestres\Semestre VI\Desarrollo Web\CODIGO\PAW-CARE-BACK\PAW-CARE-SPRINGBOOT\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB9BA15-DFA4-4497-9B13-6A9AEC79808F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFC37EF-A930-4A57-87B0-D1DEB201DC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7356" yWindow="3396" windowWidth="15684" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICAMENTOS BD FINAL" sheetId="10" r:id="rId1"/>
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:E524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,7 +2032,7 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2083,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>